<commit_message>
update for model 6
</commit_message>
<xml_diff>
--- a/noSMOTE/PCM_RF_ntree500_noSMOTE.xlsx
+++ b/noSMOTE/PCM_RF_ntree500_noSMOTE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="3320" windowWidth="25600" windowHeight="13560" tabRatio="500"/>
+    <workbookView xWindow="1120" yWindow="1060" windowWidth="25600" windowHeight="13520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -231,8 +231,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -327,7 +329,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="87">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -370,6 +372,7 @@
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -412,6 +415,7 @@
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -744,7 +748,7 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="O7" sqref="O7:R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1059,20 +1063,44 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="E7" s="5">
+        <v>100</v>
+      </c>
+      <c r="F7" s="5">
+        <v>100</v>
+      </c>
+      <c r="G7" s="5">
+        <v>100</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1</v>
+      </c>
       <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
+      <c r="J7" s="5">
+        <v>100</v>
+      </c>
+      <c r="K7" s="5">
+        <v>100</v>
+      </c>
+      <c r="L7" s="5">
+        <v>100</v>
+      </c>
+      <c r="M7" s="5">
+        <v>1</v>
+      </c>
       <c r="N7" s="5"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
+      <c r="O7" s="5">
+        <v>100</v>
+      </c>
+      <c r="P7" s="5">
+        <v>100</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>100</v>
+      </c>
+      <c r="R7" s="5">
+        <v>1</v>
+      </c>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
     </row>

</xml_diff>